<commit_message>
Finished initial modeling of Organization/Person/Membership data elements.  Ready for community members to validate and review for gaps.
</commit_message>
<xml_diff>
--- a/src/Protege Elements.xlsx
+++ b/src/Protege Elements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nclinton\Desktop\CEDS Sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\CEDS-Ontology\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D90E79-00CC-4331-9E45-5E53F248638F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB87C2D6-F85F-423D-86CB-727E93268ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="810" windowWidth="23625" windowHeight="13815" firstSheet="1" activeTab="1" xr2:uid="{76A18191-D1F9-4ED3-8CFD-DEB2DFFE6CF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="9" xr2:uid="{76A18191-D1F9-4ED3-8CFD-DEB2DFFE6CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Country Codes" sheetId="7" r:id="rId7"/>
     <sheet name="States" sheetId="8" r:id="rId8"/>
     <sheet name="State Codes" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Classes!$A$1:$J$25</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4523" uniqueCount="1583">
   <si>
     <t>Name</t>
   </si>
@@ -3743,39 +3744,6 @@
     <t>WY</t>
   </si>
   <si>
-    <t>FacilityProfitStatus</t>
-  </si>
-  <si>
-    <t>FacilityProfitStatus_ForProfit</t>
-  </si>
-  <si>
-    <t>ForProfit</t>
-  </si>
-  <si>
-    <t>For-profit facility</t>
-  </si>
-  <si>
-    <t>000834</t>
-  </si>
-  <si>
-    <t>FacilityProfitStatus_GovernmentRun</t>
-  </si>
-  <si>
-    <t>GovernmentRun</t>
-  </si>
-  <si>
-    <t>Government run facility</t>
-  </si>
-  <si>
-    <t>FacilityProfitStatus_NonProfit</t>
-  </si>
-  <si>
-    <t>NonProfit</t>
-  </si>
-  <si>
-    <t>Non-profit facility</t>
-  </si>
-  <si>
     <t>xsd:normalizedString</t>
   </si>
   <si>
@@ -4647,6 +4615,192 @@
   </si>
   <si>
     <t>001946_WorkforceProgramParticipant</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>EconomicDisadvantageStatus_No</t>
+  </si>
+  <si>
+    <t>EconomicDisadvantageStatus_Yes</t>
+  </si>
+  <si>
+    <t>EnglishLearnerStatus_No</t>
+  </si>
+  <si>
+    <t>EnglishLearnerStatus_Yes</t>
+  </si>
+  <si>
+    <t>HomelessUnaccompaniedYouthStatus_No</t>
+  </si>
+  <si>
+    <t>HomelessUnaccompaniedYouthStatus_Yes</t>
+  </si>
+  <si>
+    <t>IDEAIndicator_No</t>
+  </si>
+  <si>
+    <t>IDEAIndicator_Yes</t>
+  </si>
+  <si>
+    <t>LowIncomeStatus_No</t>
+  </si>
+  <si>
+    <t>LowIncomeStatus_Yes</t>
+  </si>
+  <si>
+    <t>MaritalStatus_Divorced</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>The person is divorced.</t>
+  </si>
+  <si>
+    <t>MaritalStatus_Married</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>The person is married.</t>
+  </si>
+  <si>
+    <t>MaritalStatus_NeverMarried</t>
+  </si>
+  <si>
+    <t>Never Married</t>
+  </si>
+  <si>
+    <t>The person has never been married.</t>
+  </si>
+  <si>
+    <t>MaritalStatus_Separated</t>
+  </si>
+  <si>
+    <t>Separated</t>
+  </si>
+  <si>
+    <t>The person is legally separated, living apart from their spouse with intentions of obtaining a divorce, or permanently or temporarily separated because of marital discord.</t>
+  </si>
+  <si>
+    <t>MaritalStatus_Widowed</t>
+  </si>
+  <si>
+    <t>Widowed</t>
+  </si>
+  <si>
+    <t>The person has lost a spouse through death.</t>
+  </si>
+  <si>
+    <t>MigrantStatus_No</t>
+  </si>
+  <si>
+    <t>MigrantStatus_Yes</t>
+  </si>
+  <si>
+    <t>PerkinsLEPStatus_No</t>
+  </si>
+  <si>
+    <t>PerkinsLEPStatus_Yes</t>
+  </si>
+  <si>
+    <t>ProfessionalAssociationMembershipStatus_No</t>
+  </si>
+  <si>
+    <t>ProfessionalAssociationMembershipStatus_Yes</t>
+  </si>
+  <si>
+    <t>PublicAssistanceStatus_No</t>
+  </si>
+  <si>
+    <t>PublicAssistanceStatus_Yes</t>
+  </si>
+  <si>
+    <t>RuralResidencyStatus_No</t>
+  </si>
+  <si>
+    <t>RuralResidencyStatus_Yes</t>
+  </si>
+  <si>
+    <t>SchoolChoiceAppliedForTransferStatus_No</t>
+  </si>
+  <si>
+    <t>SchoolChoiceAppliedForTransferStatus_Yes</t>
+  </si>
+  <si>
+    <t>SchoolChoiceEligibleForTransferStatus_No</t>
+  </si>
+  <si>
+    <t>SchoolChoiceEligibleForTransferStatus_Yes</t>
+  </si>
+  <si>
+    <t>SchoolChoiceTransferStatus_No</t>
+  </si>
+  <si>
+    <t>SchoolChoiceTransferStatus_Yes</t>
+  </si>
+  <si>
+    <t>SingleParentOrSinglePregnantWomanStatus_No</t>
+  </si>
+  <si>
+    <t>SingleParentOrSinglePregnantWomanStatus_Yes</t>
+  </si>
+  <si>
+    <t>StateApprovedTechnicalAssistanceProviderStatus_No</t>
+  </si>
+  <si>
+    <t>StateApprovedTechnicalAssistanceProviderStatus_Yes</t>
+  </si>
+  <si>
+    <t>StateApprovedTrainerStatus_No</t>
+  </si>
+  <si>
+    <t>StateApprovedTrainerStatus_Yes</t>
+  </si>
+  <si>
+    <t>TitleIIIImmigrantStatus_No</t>
+  </si>
+  <si>
+    <t>TitleIIIImmigrantStatus_Yes</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesAppliedStatus_No</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesAppliedStatus_Yes</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesEligibleStatus_No</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesEligibleStatus_Yes</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesReceivedStatus_No</t>
+  </si>
+  <si>
+    <t>TitleISchoolSupplementalServicesReceivedStatus_Yes</t>
+  </si>
+  <si>
+    <t>TruantStatus_No</t>
+  </si>
+  <si>
+    <t>TruantStatus_Yes</t>
+  </si>
+  <si>
+    <t>State Code</t>
+  </si>
+  <si>
+    <t>State Name</t>
+  </si>
+  <si>
+    <t>State ANSI Code</t>
   </si>
 </sst>
 </file>
@@ -4696,7 +4850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4704,11 +4858,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4720,6 +4887,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4735,6 +4903,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60693616-DF57-4C08-B8DF-089D5E42A209}" name="Table1" displayName="Table1" ref="A1:C58" totalsRowShown="0">
+  <autoFilter ref="A1:C58" xr:uid="{60693616-DF57-4C08-B8DF-089D5E42A209}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5D655384-AD3A-435F-93AD-00A820D8DE6B}" name="State Code"/>
+    <tableColumn id="2" xr3:uid="{59BFFC97-6E21-49D3-B38B-5BFD4CDAB4B7}" name="State Name"/>
+    <tableColumn id="3" xr3:uid="{EB7DC4F7-6B57-4BC4-926F-521B22936458}" name="State ANSI Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5087,102 +5267,102 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1243</v>
+        <v>1232</v>
       </c>
       <c r="B2" t="s">
-        <v>1244</v>
+        <v>1233</v>
       </c>
       <c r="D2" t="s">
-        <v>1245</v>
+        <v>1234</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1428</v>
+        <v>1417</v>
       </c>
       <c r="K2" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1250</v>
+        <v>1239</v>
       </c>
       <c r="B3" t="s">
-        <v>1251</v>
+        <v>1240</v>
       </c>
       <c r="D3" t="s">
-        <v>1252</v>
+        <v>1241</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1430</v>
+        <v>1419</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1253</v>
+        <v>1242</v>
       </c>
       <c r="B4" t="s">
-        <v>1254</v>
+        <v>1243</v>
       </c>
       <c r="D4" t="s">
-        <v>1255</v>
+        <v>1244</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1431</v>
+        <v>1420</v>
       </c>
       <c r="K4" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1256</v>
+        <v>1245</v>
       </c>
       <c r="B5" t="s">
-        <v>1257</v>
+        <v>1246</v>
       </c>
       <c r="D5" t="s">
-        <v>1258</v>
+        <v>1247</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>1432</v>
+        <v>1421</v>
       </c>
       <c r="K5" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1259</v>
+        <v>1248</v>
       </c>
       <c r="B6" t="s">
-        <v>1260</v>
+        <v>1249</v>
       </c>
       <c r="D6" t="s">
-        <v>1261</v>
+        <v>1250</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>1433</v>
+        <v>1422</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
@@ -5191,234 +5371,234 @@
         <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1262</v>
+        <v>1251</v>
       </c>
       <c r="B7" t="s">
-        <v>1263</v>
+        <v>1252</v>
       </c>
       <c r="D7" t="s">
-        <v>1264</v>
+        <v>1253</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>1434</v>
+        <v>1423</v>
       </c>
       <c r="K7" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1265</v>
+        <v>1254</v>
       </c>
       <c r="B8" t="s">
-        <v>1266</v>
+        <v>1255</v>
       </c>
       <c r="C8" t="s">
-        <v>1267</v>
+        <v>1256</v>
       </c>
       <c r="D8" t="s">
-        <v>1268</v>
+        <v>1257</v>
       </c>
       <c r="E8" t="s">
-        <v>1269</v>
+        <v>1258</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>1435</v>
+        <v>1424</v>
       </c>
       <c r="K8" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1270</v>
+        <v>1259</v>
       </c>
       <c r="B9" t="s">
-        <v>1271</v>
+        <v>1260</v>
       </c>
       <c r="D9" t="s">
-        <v>1272</v>
+        <v>1261</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>1436</v>
+        <v>1425</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>1273</v>
+        <v>1262</v>
       </c>
       <c r="K9" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1285</v>
+        <v>1274</v>
       </c>
       <c r="B10" t="s">
-        <v>1286</v>
+        <v>1275</v>
       </c>
       <c r="D10" t="s">
-        <v>1287</v>
+        <v>1276</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>1439</v>
+        <v>1428</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>1288</v>
+        <v>1277</v>
       </c>
       <c r="K10" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1289</v>
+        <v>1278</v>
       </c>
       <c r="B11" t="s">
-        <v>1290</v>
+        <v>1279</v>
       </c>
       <c r="D11" t="s">
-        <v>1291</v>
+        <v>1280</v>
       </c>
       <c r="E11" t="s">
-        <v>1292</v>
+        <v>1281</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>1440</v>
+        <v>1429</v>
       </c>
       <c r="K11" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1293</v>
+        <v>1282</v>
       </c>
       <c r="B12" t="s">
-        <v>1294</v>
+        <v>1283</v>
       </c>
       <c r="D12" t="s">
-        <v>1295</v>
+        <v>1284</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>1441</v>
+        <v>1430</v>
       </c>
       <c r="K12" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1296</v>
+        <v>1285</v>
       </c>
       <c r="B13" t="s">
-        <v>1297</v>
+        <v>1286</v>
       </c>
       <c r="D13" t="s">
-        <v>1298</v>
+        <v>1287</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>1442</v>
+        <v>1431</v>
       </c>
       <c r="K13" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1303</v>
+        <v>1292</v>
       </c>
       <c r="B14" t="s">
-        <v>1304</v>
+        <v>1293</v>
       </c>
       <c r="D14" t="s">
-        <v>1305</v>
+        <v>1294</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>1444</v>
+        <v>1433</v>
       </c>
       <c r="K14" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1306</v>
+        <v>1295</v>
       </c>
       <c r="B15" t="s">
-        <v>1307</v>
+        <v>1296</v>
       </c>
       <c r="D15" t="s">
-        <v>1308</v>
+        <v>1297</v>
       </c>
       <c r="E15" t="s">
-        <v>1309</v>
+        <v>1298</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>1445</v>
+        <v>1434</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>1310</v>
+        <v>1299</v>
       </c>
       <c r="K15" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1314</v>
+        <v>1303</v>
       </c>
       <c r="B16" t="s">
-        <v>1315</v>
+        <v>1304</v>
       </c>
       <c r="D16" t="s">
-        <v>1316</v>
+        <v>1305</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>1447</v>
+        <v>1436</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
@@ -5427,159 +5607,159 @@
         <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1333</v>
+        <v>1322</v>
       </c>
       <c r="B17" t="s">
-        <v>1334</v>
+        <v>1323</v>
       </c>
       <c r="D17" t="s">
-        <v>1335</v>
+        <v>1324</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>1452</v>
+        <v>1441</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1336</v>
+        <v>1325</v>
       </c>
       <c r="B18" t="s">
-        <v>1337</v>
+        <v>1326</v>
       </c>
       <c r="C18" t="s">
-        <v>1338</v>
+        <v>1327</v>
       </c>
       <c r="D18" t="s">
-        <v>1339</v>
+        <v>1328</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>1453</v>
+        <v>1442</v>
       </c>
       <c r="K18" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1340</v>
+        <v>1329</v>
       </c>
       <c r="B19" t="s">
-        <v>1341</v>
+        <v>1330</v>
       </c>
       <c r="D19" t="s">
-        <v>1342</v>
+        <v>1331</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>1454</v>
+        <v>1443</v>
       </c>
       <c r="I19" t="s">
         <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>1343</v>
+        <v>1332</v>
       </c>
       <c r="K19" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1353</v>
+        <v>1342</v>
       </c>
       <c r="B20" t="s">
-        <v>1354</v>
+        <v>1343</v>
       </c>
       <c r="D20" t="s">
-        <v>1355</v>
+        <v>1344</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>1457</v>
+        <v>1446</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="K20" t="s">
-        <v>1357</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1358</v>
+        <v>1347</v>
       </c>
       <c r="B21" t="s">
-        <v>1359</v>
+        <v>1348</v>
       </c>
       <c r="D21" t="s">
-        <v>1360</v>
+        <v>1349</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>1458</v>
+        <v>1447</v>
       </c>
       <c r="K21" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1361</v>
+        <v>1350</v>
       </c>
       <c r="B22" t="s">
-        <v>1362</v>
+        <v>1351</v>
       </c>
       <c r="D22" t="s">
-        <v>1363</v>
+        <v>1352</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>1459</v>
+        <v>1448</v>
       </c>
       <c r="K22" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1364</v>
+        <v>1353</v>
       </c>
       <c r="B23" t="s">
-        <v>1365</v>
+        <v>1354</v>
       </c>
       <c r="D23" t="s">
-        <v>1366</v>
+        <v>1355</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>1460</v>
+        <v>1449</v>
       </c>
       <c r="I23" t="s">
         <v>14</v>
@@ -5588,388 +5768,388 @@
         <v>15</v>
       </c>
       <c r="K23" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1367</v>
+        <v>1356</v>
       </c>
       <c r="B24" t="s">
-        <v>1368</v>
+        <v>1357</v>
       </c>
       <c r="D24" t="s">
-        <v>1369</v>
+        <v>1358</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>1461</v>
+        <v>1450</v>
       </c>
       <c r="K24" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1370</v>
+        <v>1359</v>
       </c>
       <c r="B25" t="s">
-        <v>1371</v>
+        <v>1360</v>
       </c>
       <c r="D25" t="s">
-        <v>1372</v>
+        <v>1361</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>1462</v>
+        <v>1451</v>
       </c>
       <c r="K25" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1373</v>
+        <v>1362</v>
       </c>
       <c r="B26" t="s">
-        <v>1374</v>
+        <v>1363</v>
       </c>
       <c r="D26" t="s">
-        <v>1375</v>
+        <v>1364</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>1463</v>
+        <v>1452</v>
       </c>
       <c r="K26" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1376</v>
+        <v>1365</v>
       </c>
       <c r="B27" t="s">
-        <v>1377</v>
+        <v>1366</v>
       </c>
       <c r="D27" t="s">
-        <v>1378</v>
+        <v>1367</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
       <c r="K27" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1379</v>
+        <v>1368</v>
       </c>
       <c r="B28" t="s">
-        <v>1380</v>
+        <v>1369</v>
       </c>
       <c r="D28" t="s">
-        <v>1381</v>
+        <v>1370</v>
       </c>
       <c r="E28" t="s">
-        <v>1382</v>
+        <v>1371</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>1465</v>
+        <v>1454</v>
       </c>
       <c r="K28" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1383</v>
+        <v>1372</v>
       </c>
       <c r="B29" t="s">
-        <v>1384</v>
+        <v>1373</v>
       </c>
       <c r="D29" t="s">
-        <v>1385</v>
+        <v>1374</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>1466</v>
+        <v>1455</v>
       </c>
       <c r="K29" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1386</v>
+        <v>1375</v>
       </c>
       <c r="B30" t="s">
-        <v>1386</v>
+        <v>1375</v>
       </c>
       <c r="D30" t="s">
-        <v>1387</v>
+        <v>1376</v>
       </c>
       <c r="E30" t="s">
-        <v>1388</v>
+        <v>1377</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>1467</v>
+        <v>1456</v>
       </c>
       <c r="K30" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1389</v>
+        <v>1378</v>
       </c>
       <c r="B31" t="s">
-        <v>1390</v>
+        <v>1379</v>
       </c>
       <c r="D31" t="s">
-        <v>1391</v>
+        <v>1380</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>1468</v>
+        <v>1457</v>
       </c>
       <c r="K31" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1392</v>
+        <v>1381</v>
       </c>
       <c r="B32" t="s">
-        <v>1393</v>
+        <v>1382</v>
       </c>
       <c r="D32" t="s">
-        <v>1394</v>
+        <v>1383</v>
       </c>
       <c r="E32" t="s">
-        <v>1395</v>
+        <v>1384</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>1469</v>
+        <v>1458</v>
       </c>
       <c r="K32" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1396</v>
+        <v>1385</v>
       </c>
       <c r="B33" t="s">
-        <v>1397</v>
+        <v>1386</v>
       </c>
       <c r="D33" t="s">
-        <v>1398</v>
+        <v>1387</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>1470</v>
+        <v>1459</v>
       </c>
       <c r="K33" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1402</v>
+        <v>1391</v>
       </c>
       <c r="B34" t="s">
-        <v>1403</v>
+        <v>1392</v>
       </c>
       <c r="D34" t="s">
-        <v>1404</v>
+        <v>1393</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>1472</v>
+        <v>1461</v>
       </c>
       <c r="K34" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1405</v>
+        <v>1394</v>
       </c>
       <c r="B35" t="s">
-        <v>1406</v>
+        <v>1395</v>
       </c>
       <c r="D35" t="s">
-        <v>1407</v>
+        <v>1396</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>1473</v>
+        <v>1462</v>
       </c>
       <c r="K35" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1408</v>
+        <v>1397</v>
       </c>
       <c r="B36" t="s">
-        <v>1409</v>
+        <v>1398</v>
       </c>
       <c r="D36" t="s">
-        <v>1410</v>
+        <v>1399</v>
       </c>
       <c r="F36" t="s">
         <v>10</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>1474</v>
+        <v>1463</v>
       </c>
       <c r="K36" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1411</v>
+        <v>1400</v>
       </c>
       <c r="B37" t="s">
-        <v>1412</v>
+        <v>1401</v>
       </c>
       <c r="D37" t="s">
-        <v>1413</v>
+        <v>1402</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>1475</v>
+        <v>1464</v>
       </c>
       <c r="K37" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1414</v>
+        <v>1403</v>
       </c>
       <c r="B38" t="s">
-        <v>1415</v>
+        <v>1404</v>
       </c>
       <c r="D38" t="s">
-        <v>1416</v>
+        <v>1405</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>1476</v>
+        <v>1465</v>
       </c>
       <c r="I38" t="s">
         <v>14</v>
       </c>
       <c r="J38" t="s">
-        <v>1417</v>
+        <v>1406</v>
       </c>
       <c r="K38" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1418</v>
+        <v>1407</v>
       </c>
       <c r="B39" t="s">
-        <v>1419</v>
+        <v>1408</v>
       </c>
       <c r="D39" t="s">
-        <v>1420</v>
+        <v>1409</v>
       </c>
       <c r="E39" t="s">
-        <v>1421</v>
+        <v>1410</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>1477</v>
+        <v>1466</v>
       </c>
       <c r="K39" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1422</v>
+        <v>1411</v>
       </c>
       <c r="B40" t="s">
-        <v>1423</v>
+        <v>1412</v>
       </c>
       <c r="D40" t="s">
-        <v>1424</v>
+        <v>1413</v>
       </c>
       <c r="E40" t="s">
-        <v>1388</v>
+        <v>1377</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>1478</v>
+        <v>1467</v>
       </c>
       <c r="K40" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1425</v>
+        <v>1414</v>
       </c>
       <c r="B41" t="s">
-        <v>1426</v>
+        <v>1415</v>
       </c>
       <c r="D41" t="s">
-        <v>1427</v>
+        <v>1416</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>1479</v>
+        <v>1468</v>
       </c>
       <c r="K41" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
     </row>
   </sheetData>
@@ -5979,11 +6159,674 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7A7535-24A8-4439-B299-D20B4EB2C230}">
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>827</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>831</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>832</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>837</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>859</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>878</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>894</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>897</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>913</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>922</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>924</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>926</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>945</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>947</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>958</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>960</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>961</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>964</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>968</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>969</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>973</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>974</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>982</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>983</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>994</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B46" t="s">
+        <v>507</v>
+      </c>
+      <c r="C46">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B51" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E975D21-BCFB-4BD5-B09E-D59073294458}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6017,233 +6860,233 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B2" t="s">
-        <v>1481</v>
+        <v>1470</v>
       </c>
       <c r="C2" t="s">
-        <v>1482</v>
+        <v>1471</v>
       </c>
       <c r="D2" t="s">
-        <v>1483</v>
+        <v>1472</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>1484</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B3" t="s">
-        <v>1485</v>
+        <v>1474</v>
       </c>
       <c r="C3" t="s">
-        <v>1486</v>
+        <v>1475</v>
       </c>
       <c r="D3" t="s">
-        <v>1487</v>
+        <v>1476</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>1488</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D4" t="s">
         <v>1480</v>
       </c>
-      <c r="B4" t="s">
-        <v>1489</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1490</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1491</v>
-      </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>1492</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B5" t="s">
-        <v>1493</v>
+        <v>1482</v>
       </c>
       <c r="C5" t="s">
-        <v>1494</v>
+        <v>1483</v>
       </c>
       <c r="D5" t="s">
-        <v>1495</v>
+        <v>1484</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>1496</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B6" t="s">
-        <v>1497</v>
+        <v>1486</v>
       </c>
       <c r="C6" t="s">
-        <v>1498</v>
+        <v>1487</v>
       </c>
       <c r="D6" t="s">
-        <v>1499</v>
+        <v>1488</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>1500</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B7" t="s">
-        <v>1501</v>
+        <v>1490</v>
       </c>
       <c r="C7" t="s">
-        <v>1502</v>
+        <v>1491</v>
       </c>
       <c r="D7" t="s">
-        <v>1503</v>
+        <v>1492</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>1504</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B8" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="C8" t="s">
-        <v>1506</v>
+        <v>1495</v>
       </c>
       <c r="D8" t="s">
-        <v>1507</v>
+        <v>1496</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>1508</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B9" t="s">
-        <v>1509</v>
+        <v>1498</v>
       </c>
       <c r="C9" t="s">
-        <v>1510</v>
+        <v>1499</v>
       </c>
       <c r="D9" t="s">
-        <v>1511</v>
+        <v>1500</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>1512</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B10" t="s">
-        <v>1513</v>
+        <v>1502</v>
       </c>
       <c r="C10" t="s">
-        <v>1514</v>
+        <v>1503</v>
       </c>
       <c r="D10" t="s">
-        <v>1515</v>
+        <v>1504</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>1516</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B11" t="s">
-        <v>1517</v>
+        <v>1506</v>
       </c>
       <c r="C11" t="s">
-        <v>1518</v>
+        <v>1507</v>
       </c>
       <c r="D11" t="s">
-        <v>1519</v>
+        <v>1508</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>1520</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B12" t="s">
-        <v>1521</v>
+        <v>1510</v>
       </c>
       <c r="C12" t="s">
-        <v>1522</v>
+        <v>1511</v>
       </c>
       <c r="D12" t="s">
-        <v>1523</v>
+        <v>1512</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>1524</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B13" t="s">
-        <v>1525</v>
+        <v>1514</v>
       </c>
       <c r="C13" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
@@ -6252,27 +7095,27 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>1527</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1480</v>
+        <v>1469</v>
       </c>
       <c r="B14" t="s">
-        <v>1528</v>
+        <v>1517</v>
       </c>
       <c r="C14" t="s">
-        <v>1529</v>
+        <v>1518</v>
       </c>
       <c r="D14" t="s">
-        <v>1530</v>
+        <v>1519</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>1531</v>
+        <v>1520</v>
       </c>
     </row>
   </sheetData>
@@ -6339,19 +7182,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1246</v>
+        <v>1235</v>
       </c>
       <c r="B2" t="s">
-        <v>1246</v>
+        <v>1235</v>
       </c>
       <c r="D2" t="s">
-        <v>1247</v>
+        <v>1236</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1429</v>
+        <v>1418</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
@@ -6360,285 +7203,285 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>1248</v>
+        <v>1237</v>
       </c>
       <c r="K2" t="s">
-        <v>1249</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1274</v>
+        <v>1263</v>
       </c>
       <c r="B3" t="s">
-        <v>1275</v>
+        <v>1264</v>
       </c>
       <c r="D3" t="s">
-        <v>1276</v>
+        <v>1265</v>
       </c>
       <c r="E3" t="s">
-        <v>1277</v>
+        <v>1266</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1437</v>
+        <v>1426</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1278</v>
+        <v>1267</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>1279</v>
+        <v>1268</v>
       </c>
       <c r="K3" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1280</v>
+        <v>1269</v>
       </c>
       <c r="B4" t="s">
-        <v>1281</v>
+        <v>1270</v>
       </c>
       <c r="D4" t="s">
-        <v>1282</v>
+        <v>1271</v>
       </c>
       <c r="E4" t="s">
-        <v>1283</v>
+        <v>1272</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1438</v>
+        <v>1427</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>1284</v>
+        <v>1273</v>
       </c>
       <c r="K4" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1299</v>
+        <v>1288</v>
       </c>
       <c r="B5" t="s">
-        <v>1300</v>
+        <v>1289</v>
       </c>
       <c r="C5" t="s">
-        <v>1301</v>
+        <v>1290</v>
       </c>
       <c r="D5" t="s">
-        <v>1302</v>
+        <v>1291</v>
       </c>
       <c r="E5" t="s">
-        <v>1283</v>
+        <v>1272</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>1443</v>
+        <v>1432</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>1278</v>
+        <v>1267</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>1279</v>
+        <v>1268</v>
       </c>
       <c r="K5" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1311</v>
+        <v>1300</v>
       </c>
       <c r="B6" t="s">
-        <v>1312</v>
+        <v>1301</v>
       </c>
       <c r="D6" t="s">
-        <v>1313</v>
+        <v>1302</v>
       </c>
       <c r="E6" t="s">
-        <v>1283</v>
+        <v>1272</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>1446</v>
+        <v>1435</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>1278</v>
+        <v>1267</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>1279</v>
+        <v>1268</v>
       </c>
       <c r="K6" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1317</v>
+        <v>1306</v>
       </c>
       <c r="B7" t="s">
-        <v>1318</v>
+        <v>1307</v>
       </c>
       <c r="D7" t="s">
-        <v>1319</v>
+        <v>1308</v>
       </c>
       <c r="E7" t="s">
-        <v>1320</v>
+        <v>1309</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>1448</v>
+        <v>1437</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>1321</v>
+        <v>1310</v>
       </c>
       <c r="K7" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1322</v>
+        <v>1311</v>
       </c>
       <c r="B8" t="s">
-        <v>1323</v>
+        <v>1312</v>
       </c>
       <c r="D8" t="s">
-        <v>1324</v>
+        <v>1313</v>
       </c>
       <c r="E8" t="s">
-        <v>1325</v>
+        <v>1314</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>1449</v>
+        <v>1438</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>1321</v>
+        <v>1310</v>
       </c>
       <c r="K8" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1326</v>
+        <v>1315</v>
       </c>
       <c r="B9" t="s">
-        <v>1327</v>
+        <v>1316</v>
       </c>
       <c r="D9" t="s">
-        <v>1328</v>
+        <v>1317</v>
       </c>
       <c r="E9" t="s">
-        <v>1329</v>
+        <v>1318</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>1450</v>
+        <v>1439</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>1321</v>
+        <v>1310</v>
       </c>
       <c r="K9" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1330</v>
+        <v>1319</v>
       </c>
       <c r="B10" t="s">
-        <v>1331</v>
+        <v>1320</v>
       </c>
       <c r="D10" t="s">
-        <v>1332</v>
+        <v>1321</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>1451</v>
+        <v>1440</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1344</v>
+        <v>1333</v>
       </c>
       <c r="B11" t="s">
-        <v>1345</v>
+        <v>1334</v>
       </c>
       <c r="C11" t="s">
-        <v>1346</v>
+        <v>1335</v>
       </c>
       <c r="D11" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>1455</v>
+        <v>1444</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1348</v>
+        <v>1337</v>
       </c>
       <c r="B12" t="s">
-        <v>1349</v>
+        <v>1338</v>
       </c>
       <c r="D12" t="s">
-        <v>1350</v>
+        <v>1339</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>1456</v>
+        <v>1445</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>1351</v>
+        <v>1340</v>
       </c>
       <c r="K12" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -6877,19 +7720,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1399</v>
+        <v>1388</v>
       </c>
       <c r="B2" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
       <c r="D2" t="s">
-        <v>1401</v>
+        <v>1390</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1471</v>
+        <v>1460</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -6906,9 +7749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9500FC2-887E-4353-8536-496DB861D87F}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6945,72 +7786,1084 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1233</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1234</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="A2" s="11" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11">
+        <v>180</v>
+      </c>
+      <c r="G2" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="11">
+        <v>180</v>
+      </c>
+      <c r="G3" s="11">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1236</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1237</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1234</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1230</v>
+        <v>1282</v>
       </c>
       <c r="B4" t="s">
-        <v>1238</v>
+        <v>1527</v>
       </c>
       <c r="C4" t="s">
-        <v>1239</v>
+        <v>1521</v>
       </c>
       <c r="D4" t="s">
-        <v>1240</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1234</v>
+        <v>1430</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G45" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="G47" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="G48" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
@@ -20806,7 +22659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF86352A-937C-455D-8F27-FB150FF44249}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>